<commit_message>
WAITM-617 Rounding as a number instead of a string
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-vitals-sensitive-true.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-vitals-sensitive-true.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD40CFE0-6549-644E-9CEA-5546544C5144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60054E2A-DD48-7243-8312-EDC0D1EEECED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>(PatientVitalsWeight/PatientVitalsHeight/PatientVitalsHeight)*10000</t>
   </si>
   <si>
-    <t>{"rounding": "1"}</t>
-  </si>
-  <si>
     <t>pde-PatientVitalsSBP</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>{"min": 32, "max": 44, "normalRange": {"min": 35.5, "max": 37.5}}</t>
   </si>
   <si>
-    <t>{"unit": "°C", "rounding": "1"}</t>
-  </si>
-  <si>
     <t>pde-PatientVitalsSPO2</t>
   </si>
   <si>
@@ -355,6 +349,12 @@
   </si>
   <si>
     <t>Vitals-sensitive</t>
+  </si>
+  <si>
+    <t>{"rounding": 1}</t>
+  </si>
+  <si>
+    <t>{"unit": "°C", "rounding": 1}</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -784,7 +784,7 @@
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1961,254 +1961,254 @@
         <v>52</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="Q11" s="2" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>